<commit_message>
Refactor scripts to use consistent PSModulesPath and improve S3 bucket creation logic; add advanced userdata script for EC2 configuration and DynamoDB table creation for Terraform state locking.
</commit_message>
<xml_diff>
--- a/EC2_Config.xlsx
+++ b/EC2_Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\aws-new\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED1E76ED-9F71-4AA7-8A30-BE7EF69C11B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD064647-D044-4961-A425-63CEBFB72CBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3585" yWindow="3585" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ec2_instances" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="115">
   <si>
     <t>SSORole</t>
   </si>
@@ -138,9 +138,6 @@
   </si>
   <si>
     <t>Tags</t>
-  </si>
-  <si>
-    <t>UserData</t>
   </si>
   <si>
     <t>Domain</t>
@@ -780,10 +777,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:AL2"/>
+  <dimension ref="A1:AK2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="AJ13" sqref="AJ13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,16 +817,15 @@
     <col min="31" max="31" width="14" style="5" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="15" style="5" customWidth="1"/>
     <col min="33" max="33" width="55.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="32.140625" style="5" customWidth="1"/>
-    <col min="35" max="35" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="15.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="14" style="5" bestFit="1" customWidth="1"/>
-    <col min="39" max="51" width="14.7109375" style="5" customWidth="1"/>
-    <col min="52" max="16384" width="14.7109375" style="5"/>
+    <col min="34" max="34" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="15.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="14" style="5" bestFit="1" customWidth="1"/>
+    <col min="38" max="50" width="14.7109375" style="5" customWidth="1"/>
+    <col min="51" max="16384" width="14.7109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -941,52 +937,49 @@
       <c r="AK1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:37" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:38" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="B2" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="C2" s="9">
         <v>222482127286</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>46</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>47</v>
       </c>
       <c r="L2" s="5" t="b">
         <v>0</v>
       </c>
       <c r="M2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="N2" s="5" t="s">
         <v>48</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>49</v>
       </c>
       <c r="O2" s="5" t="b">
         <v>0</v>
@@ -995,7 +988,7 @@
         <v>30</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="R2" s="5" t="b">
         <v>1</v>
@@ -1004,10 +997,10 @@
         <v>0</v>
       </c>
       <c r="U2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="V2" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="V2" s="5" t="s">
-        <v>52</v>
       </c>
       <c r="W2" s="5">
         <v>1</v>
@@ -1019,13 +1012,13 @@
         <v>1</v>
       </c>
       <c r="Z2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA2" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="AA2" s="5" t="s">
+      <c r="AB2" s="5" t="s">
         <v>54</v>
-      </c>
-      <c r="AB2" s="5" t="s">
-        <v>55</v>
       </c>
       <c r="AC2" s="5" t="b">
         <v>0</v>
@@ -1034,10 +1027,10 @@
         <v>0</v>
       </c>
       <c r="AG2" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH2" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="AI2" s="5" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1049,7 +1042,7 @@
           <x14:formula1>
             <xm:f>lookup!$A$2:$A$7</xm:f>
           </x14:formula1>
-          <xm:sqref>AI2:AL2</xm:sqref>
+          <xm:sqref>AH2:AK2</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{439A3BFE-EEA8-448F-83E7-52A03BA69347}">
           <x14:formula1>
@@ -1082,7 +1075,7 @@
   </sheetPr>
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
@@ -1103,7 +1096,7 @@
     <col min="14" max="14" width="17.85546875" customWidth="1"/>
     <col min="15" max="15" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="34.28515625" customWidth="1"/>
+    <col min="17" max="17" width="44.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1120,28 +1113,28 @@
         <v>3</v>
       </c>
       <c r="E1" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>64</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>65</v>
       </c>
       <c r="M1" s="7" t="s">
         <v>17</v>
@@ -1150,10 +1143,10 @@
         <v>18</v>
       </c>
       <c r="O1" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="P1" s="7" t="s">
         <v>66</v>
-      </c>
-      <c r="P1" s="7" t="s">
-        <v>67</v>
       </c>
       <c r="Q1" s="7" t="s">
         <v>32</v>
@@ -1161,34 +1154,34 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="9">
         <v>222482127286</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
         <v>39</v>
       </c>
-      <c r="D2" t="s">
-        <v>40</v>
-      </c>
       <c r="E2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G2">
         <v>100</v>
       </c>
       <c r="H2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J2" t="s">
         <v>69</v>
-      </c>
-      <c r="J2" t="s">
-        <v>70</v>
       </c>
       <c r="K2">
         <v>4000</v>
@@ -1216,7 +1209,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4E325C2-9FA0-4B3C-803E-A16465821B7B}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -1243,24 +1236,24 @@
         <v>4</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="C2" s="9">
         <v>222482127286</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1306,25 +1299,25 @@
         <v>3</v>
       </c>
       <c r="E1" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>77</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>78</v>
       </c>
       <c r="L1" s="7" t="s">
         <v>32</v>
@@ -1332,78 +1325,78 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="2">
         <v>222482127286</v>
       </c>
       <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
         <v>39</v>
       </c>
-      <c r="D2" t="s">
-        <v>40</v>
-      </c>
       <c r="E2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" t="s">
         <v>79</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>80</v>
-      </c>
-      <c r="G2" t="s">
-        <v>81</v>
       </c>
       <c r="H2">
         <v>5</v>
       </c>
       <c r="I2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J2" t="s">
         <v>82</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>83</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>84</v>
-      </c>
-      <c r="L2" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" s="2">
         <v>222482127286</v>
       </c>
       <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
         <v>39</v>
       </c>
-      <c r="D3" t="s">
-        <v>40</v>
-      </c>
       <c r="E3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" t="s">
         <v>79</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>80</v>
-      </c>
-      <c r="G3" t="s">
-        <v>81</v>
       </c>
       <c r="H3">
         <v>5</v>
       </c>
       <c r="I3" t="s">
+        <v>85</v>
+      </c>
+      <c r="J3" t="s">
         <v>86</v>
       </c>
-      <c r="J3" t="s">
-        <v>87</v>
-      </c>
       <c r="K3" t="s">
+        <v>83</v>
+      </c>
+      <c r="L3" t="s">
         <v>84</v>
-      </c>
-      <c r="L3" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1451,31 +1444,31 @@
         <v>1</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="J1" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="K1" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>95</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>96</v>
       </c>
       <c r="M1" s="4" t="s">
         <v>32</v>
@@ -1486,28 +1479,28 @@
     </row>
     <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="9">
         <v>222482127286</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>99</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>100</v>
       </c>
       <c r="I2" s="11">
         <v>80</v>
@@ -1516,42 +1509,42 @@
         <v>80</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L2" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="N2" t="s">
         <v>101</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="N2" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" s="9">
         <v>222482127286</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D3" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>99</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>100</v>
       </c>
       <c r="I3" s="11">
         <v>443</v>
@@ -1560,42 +1553,42 @@
         <v>443</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" s="9">
         <v>222482127286</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="G4" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>99</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>100</v>
       </c>
       <c r="I4" s="11">
         <v>22</v>
@@ -1604,42 +1597,42 @@
         <v>22</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="9">
         <v>222482127286</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D5" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="G5" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>99</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>100</v>
       </c>
       <c r="I5" s="11">
         <v>5723</v>
@@ -1648,16 +1641,16 @@
         <v>5723</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1700,10 +1693,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>5</v>
@@ -1712,38 +1705,38 @@
         <v>4</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="9">
         <v>222482127286</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
         <v>39</v>
-      </c>
-      <c r="D2" t="s">
-        <v>40</v>
       </c>
       <c r="E2" t="str">
         <f>sg_rules!F2</f>
         <v>vpc-0b33c6cf3b601d4db</v>
       </c>
       <c r="F2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G2" t="str">
         <f>ec2_instances!F2</f>
         <v>az1autoprod-vm</v>
       </c>
       <c r="H2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1769,7 +1762,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>25</v>
@@ -1783,50 +1776,50 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
         <v>108</v>
-      </c>
-      <c r="B2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" t="s">
         <v>110</v>
       </c>
-      <c r="B3" t="s">
-        <v>111</v>
-      </c>
       <c r="C3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement modular Windows EC2 bootstrapping framework with S3-based configuration and PowerShell scripts
- Added Bootstrap.md documentation outlining the bootstrapping process and prerequisites.
- Created Bootstrap.ps1 as the main entry point for EC2 instance configuration.
- Developed Bootstrap_v2.ps1 with enhanced logging and error handling for instance setup.
- Introduced Config.json for instance-specific configurations including networking and EBS volumes.
- Implemented Initialize-AndFormatDisks.ps1 for disk initialization and formatting.
- Added Install-SQL.ps1 for SQL Server installation based on configuration.
- Created Join-Domain.ps1 for domain joining functionality with secure credential retrieval.
- Developed Rename-Computer.ps1 for safe computer renaming.
- Implemented Set-Network.ps1 for static IP configuration.
- Created Startup.ps1 for post-reboot actions including SQL installation.
- Added EC2 instance key pair az1cwkad01-kp.pem for secure access.
</commit_message>
<xml_diff>
--- a/EC2_Config.xlsx
+++ b/EC2_Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\aws-new\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD064647-D044-4961-A425-63CEBFB72CBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B13825-0700-4B37-ADB3-EA4308C87FAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ec2_instances" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="130">
   <si>
     <t>SSORole</t>
   </si>
@@ -146,12 +146,24 @@
     <t>DefaultGateway</t>
   </si>
   <si>
+    <t>SubnetMask</t>
+  </si>
+  <si>
     <t>PrimaryDNS</t>
   </si>
   <si>
     <t>SecondaryDNS</t>
   </si>
   <si>
+    <t>OU</t>
+  </si>
+  <si>
+    <t>SQLInstall</t>
+  </si>
+  <si>
+    <t>AppInstall</t>
+  </si>
+  <si>
     <t>AdministratorAccess</t>
   </si>
   <si>
@@ -161,236 +173,270 @@
     <t>eu-west-1a</t>
   </si>
   <si>
+    <t>az1autoprod-vm</t>
+  </si>
+  <si>
+    <t>ami-0440a5f5e96917e8f</t>
+  </si>
+  <si>
+    <t>t3.micro</t>
+  </si>
+  <si>
+    <t>autoprod-vm-keypair</t>
+  </si>
+  <si>
+    <t>subnet-044949704b137ec32</t>
+  </si>
+  <si>
+    <t>172.31.1.10</t>
+  </si>
+  <si>
+    <t>sg-0f98c1a2a752ca15d,
+sg-0e5df311e23ecdb02</t>
+  </si>
+  <si>
+    <t>iamrole-cloudwickprod-ec2</t>
+  </si>
+  <si>
+    <t>gp3</t>
+  </si>
+  <si>
+    <t>required</t>
+  </si>
+  <si>
+    <t>enabled</t>
+  </si>
+  <si>
+    <t>stop</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>hostname=az1autoprod-vm,solution=script_test</t>
+  </si>
+  <si>
+    <t>cloudwick.local</t>
+  </si>
+  <si>
+    <t>Instance</t>
+  </si>
+  <si>
+    <t>VolumeName</t>
+  </si>
+  <si>
+    <t>VolumeID</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>VolumeType</t>
+  </si>
+  <si>
+    <t>Iops</t>
+  </si>
+  <si>
+    <t>Throughput</t>
+  </si>
+  <si>
+    <t>SnapshotId</t>
+  </si>
+  <si>
+    <t>MultiAttachEnabled</t>
+  </si>
+  <si>
+    <t>PartitionStyle</t>
+  </si>
+  <si>
+    <t>VolumeMount</t>
+  </si>
+  <si>
+    <t>VolumeLabel</t>
+  </si>
+  <si>
+    <t>FileSystem</t>
+  </si>
+  <si>
+    <t>AllocationUnitSize</t>
+  </si>
+  <si>
+    <t>ebs-az1autoprod-vm-01</t>
+  </si>
+  <si>
+    <t>GPT</t>
+  </si>
+  <si>
+    <t>D:</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>NTFS</t>
+  </si>
+  <si>
+    <t>ebs-az1autoprod-vm-02</t>
+  </si>
+  <si>
+    <t>st1</t>
+  </si>
+  <si>
+    <t>E:</t>
+  </si>
+  <si>
+    <t>Backup</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
     <t>i-03ddf5c1739bde768</t>
   </si>
   <si>
-    <t>az1autoprod-vm</t>
-  </si>
-  <si>
-    <t>ami-0440a5f5e96917e8f</t>
-  </si>
-  <si>
-    <t>t3.micro</t>
-  </si>
-  <si>
-    <t>autoprod-vm-keypair</t>
-  </si>
-  <si>
-    <t>subnet-044949704b137ec32</t>
-  </si>
-  <si>
-    <t>172.31.1.10</t>
-  </si>
-  <si>
-    <t>sg-0f98c1a2a752ca15d,sg-0e5df311e23ecdb02</t>
-  </si>
-  <si>
-    <t>iamrole-cloudwickprod-ec2</t>
-  </si>
-  <si>
-    <t>gp3</t>
-  </si>
-  <si>
-    <t>required</t>
-  </si>
-  <si>
-    <t>enabled</t>
-  </si>
-  <si>
-    <t>stop</t>
-  </si>
-  <si>
-    <t>default</t>
-  </si>
-  <si>
-    <t>none</t>
-  </si>
-  <si>
-    <t>hostname=az1autoprod-vm,solution=script_test</t>
+    <t>eu-west-1</t>
+  </si>
+  <si>
+    <t>VpcID</t>
+  </si>
+  <si>
+    <t>PrefixListName</t>
+  </si>
+  <si>
+    <t>PLDescription</t>
+  </si>
+  <si>
+    <t>MaxEntries</t>
+  </si>
+  <si>
+    <t>CIDR</t>
+  </si>
+  <si>
+    <t>CIDRDescription</t>
+  </si>
+  <si>
+    <t>PrefixListId</t>
+  </si>
+  <si>
+    <t>vpc-0b33c6cf3b601d4db</t>
+  </si>
+  <si>
+    <t>prod-dmz-cidrs</t>
+  </si>
+  <si>
+    <t>DMZ CIDRs</t>
+  </si>
+  <si>
+    <t>10.0.0.0/16</t>
+  </si>
+  <si>
+    <t>Production Network</t>
+  </si>
+  <si>
+    <t>pl-0bc1a4e780a356cd5</t>
+  </si>
+  <si>
+    <t>solution=script_test</t>
+  </si>
+  <si>
+    <t>192.168.0.0/16</t>
+  </si>
+  <si>
+    <t>Home Network</t>
+  </si>
+  <si>
+    <t>GroupName</t>
+  </si>
+  <si>
+    <t>GroupDescription</t>
+  </si>
+  <si>
+    <t>VpcId</t>
+  </si>
+  <si>
+    <t>RuleType</t>
+  </si>
+  <si>
+    <t>Protocol</t>
+  </si>
+  <si>
+    <t>FromPort</t>
+  </si>
+  <si>
+    <t>ToPort</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>cloudwickprod-webserver</t>
+  </si>
+  <si>
+    <t>Security group for web servers</t>
+  </si>
+  <si>
+    <t>ingress</t>
+  </si>
+  <si>
+    <t>tcp</t>
+  </si>
+  <si>
+    <t>HTTP access from internet</t>
+  </si>
+  <si>
+    <t>sg-04df5f9ed71629ac5</t>
+  </si>
+  <si>
+    <t>HTTPS access from internet</t>
+  </si>
+  <si>
+    <t>SSH access from VPC</t>
+  </si>
+  <si>
+    <t>SCOM access from VPC</t>
+  </si>
+  <si>
+    <t>SecurityGroupNames</t>
+  </si>
+  <si>
+    <t>AttachedSecurityGroupIds</t>
+  </si>
+  <si>
+    <t>pfgroup.prvfin.com</t>
+  </si>
+  <si>
+    <t>simple</t>
+  </si>
+  <si>
+    <t>ie.pfgroup.provfin.com</t>
+  </si>
+  <si>
+    <t>terminate</t>
+  </si>
+  <si>
+    <t>prod01.local</t>
+  </si>
+  <si>
+    <t>prod02.local</t>
+  </si>
+  <si>
+    <t>uk.providentinternational.com</t>
   </si>
   <si>
     <t>workgroup</t>
-  </si>
-  <si>
-    <t>Instance</t>
-  </si>
-  <si>
-    <t>VolumeName</t>
-  </si>
-  <si>
-    <t>Size</t>
-  </si>
-  <si>
-    <t>VolumeType</t>
-  </si>
-  <si>
-    <t>VolumeMount</t>
-  </si>
-  <si>
-    <t>VolumeLabel</t>
-  </si>
-  <si>
-    <t>Iops</t>
-  </si>
-  <si>
-    <t>Throughput</t>
-  </si>
-  <si>
-    <t>SnapshotId</t>
-  </si>
-  <si>
-    <t>MultiAttachEnabled</t>
-  </si>
-  <si>
-    <t>ebs-az1autoprod-vm-01</t>
-  </si>
-  <si>
-    <t>D:</t>
-  </si>
-  <si>
-    <t>Data</t>
-  </si>
-  <si>
-    <t>Region</t>
-  </si>
-  <si>
-    <t>VpcID</t>
-  </si>
-  <si>
-    <t>PrefixListName</t>
-  </si>
-  <si>
-    <t>PLDescription</t>
-  </si>
-  <si>
-    <t>MaxEntries</t>
-  </si>
-  <si>
-    <t>CIDR</t>
-  </si>
-  <si>
-    <t>CIDRDescription</t>
-  </si>
-  <si>
-    <t>PrefixListId</t>
-  </si>
-  <si>
-    <t>vpc-0b33c6cf3b601d4db</t>
-  </si>
-  <si>
-    <t>prod-dmz-cidrs</t>
-  </si>
-  <si>
-    <t>DMZ CIDRs</t>
-  </si>
-  <si>
-    <t>10.0.0.0/16</t>
-  </si>
-  <si>
-    <t>Production Network</t>
-  </si>
-  <si>
-    <t>pl-0bc1a4e780a356cd5</t>
-  </si>
-  <si>
-    <t>solution=script_test</t>
-  </si>
-  <si>
-    <t>192.168.0.0/16</t>
-  </si>
-  <si>
-    <t>Home Network</t>
-  </si>
-  <si>
-    <t>GroupName</t>
-  </si>
-  <si>
-    <t>GroupDescription</t>
-  </si>
-  <si>
-    <t>VpcId</t>
-  </si>
-  <si>
-    <t>RuleType</t>
-  </si>
-  <si>
-    <t>Protocol</t>
-  </si>
-  <si>
-    <t>FromPort</t>
-  </si>
-  <si>
-    <t>ToPort</t>
-  </si>
-  <si>
-    <t>Source</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>cloudwickprod-webserver</t>
-  </si>
-  <si>
-    <t>Security group for web servers</t>
-  </si>
-  <si>
-    <t>ingress</t>
-  </si>
-  <si>
-    <t>tcp</t>
-  </si>
-  <si>
-    <t>HTTP access from internet</t>
-  </si>
-  <si>
-    <t>sg-04df5f9ed71629ac5</t>
-  </si>
-  <si>
-    <t>HTTPS access from internet</t>
-  </si>
-  <si>
-    <t>SSH access from VPC</t>
-  </si>
-  <si>
-    <t>SCOM access from VPC</t>
-  </si>
-  <si>
-    <t>SecurityGroupNames</t>
-  </si>
-  <si>
-    <t>AttachedSecurityGroupIds</t>
-  </si>
-  <si>
-    <t>pfgroup.prvfin.com</t>
-  </si>
-  <si>
-    <t>simple</t>
-  </si>
-  <si>
-    <t>ie.pfgroup.provfin.com</t>
-  </si>
-  <si>
-    <t>terminate</t>
-  </si>
-  <si>
-    <t>prod01.local</t>
-  </si>
-  <si>
-    <t>prod02.local</t>
-  </si>
-  <si>
-    <t>uk.providentinternational.com</t>
-  </si>
-  <si>
-    <t>eu-west-1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -419,13 +465,51 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -447,7 +531,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -472,6 +556,21 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -777,10 +876,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:AK2"/>
+  <dimension ref="A1:AO2"/>
   <sheetViews>
-    <sheetView topLeftCell="AE1" workbookViewId="0">
-      <selection activeCell="AJ13" sqref="AJ13"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="Y8" sqref="Y8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,7 +907,7 @@
     <col min="22" max="22" width="20.42578125" style="5" customWidth="1"/>
     <col min="23" max="23" width="41" style="5" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="29.7109375" style="5" customWidth="1"/>
-    <col min="25" max="25" width="19.7109375" style="5" customWidth="1"/>
+    <col min="25" max="25" width="24.85546875" style="5" customWidth="1"/>
     <col min="26" max="26" width="33.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="15.85546875" style="5" bestFit="1" customWidth="1"/>
@@ -817,169 +916,180 @@
     <col min="31" max="31" width="14" style="5" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="15" style="5" customWidth="1"/>
     <col min="33" max="33" width="55.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="15.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="14" style="5" bestFit="1" customWidth="1"/>
-    <col min="38" max="50" width="14.7109375" style="5" customWidth="1"/>
-    <col min="51" max="16384" width="14.7109375" style="5"/>
+    <col min="36" max="36" width="11.85546875" style="5" customWidth="1"/>
+    <col min="37" max="37" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14" style="5" bestFit="1" customWidth="1"/>
+    <col min="39" max="40" width="14" style="5" customWidth="1"/>
+    <col min="41" max="63" width="14.7109375" style="5" customWidth="1"/>
+    <col min="64" max="16384" width="14.7109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:41" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="U1" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="V1" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="W1" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="X1" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Y1" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="Z1" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AA1" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AB1" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AC1" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AD1" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AE1" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AF1" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AG1" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AH1" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AI1" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AJ1" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AK1" s="22" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:37" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AL1" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:41" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C2" s="9">
         <v>222482127286</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L2" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="M2" s="5" t="s">
-        <v>47</v>
+      <c r="M2" s="14" t="s">
+        <v>50</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="O2" s="5" t="b">
         <v>0</v>
@@ -988,7 +1098,7 @@
         <v>30</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="R2" s="5" t="b">
         <v>1</v>
@@ -997,10 +1107,10 @@
         <v>0</v>
       </c>
       <c r="U2" s="5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="V2" s="5" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="W2" s="5">
         <v>1</v>
@@ -1012,13 +1122,13 @@
         <v>1</v>
       </c>
       <c r="Z2" s="5" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="AA2" s="5" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="AB2" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="AC2" s="5" t="b">
         <v>0</v>
@@ -1027,10 +1137,16 @@
         <v>0</v>
       </c>
       <c r="AG2" s="5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="AH2" s="5" t="s">
-        <v>56</v>
+        <v>59</v>
+      </c>
+      <c r="AN2" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO2" s="5" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1038,12 +1154,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{31A2719D-7A9B-43DD-B9CF-8C58CDF19886}">
-          <x14:formula1>
-            <xm:f>lookup!$A$2:$A$7</xm:f>
-          </x14:formula1>
-          <xm:sqref>AH2:AK2</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{439A3BFE-EEA8-448F-83E7-52A03BA69347}">
           <x14:formula1>
             <xm:f>lookup!$B$2:$B$3</xm:f>
@@ -1062,6 +1172,12 @@
           </x14:formula1>
           <xm:sqref>AB2</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4AD6EAB3-9EA0-4BF9-B55B-8A98B88AF2E4}">
+          <x14:formula1>
+            <xm:f>lookup!$A$2:$A$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>AH2:AJ2</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -1073,10 +1189,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1087,117 +1203,192 @@
     <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.85546875" customWidth="1"/>
-    <col min="15" max="15" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="44.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="2"/>
+    <col min="11" max="11" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.85546875" customWidth="1"/>
+    <col min="14" max="14" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="0" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.42578125" customWidth="1"/>
+    <col min="21" max="21" width="17.7109375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="H1" s="7" t="s">
+      <c r="E1" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="F1" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="G1" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="H1" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="I1" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="J1" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="K1" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="M1" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="P1" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q1" s="7" t="s">
+      <c r="N1" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="O1" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="P1" s="12" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q1" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="R1" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="S1" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="T1" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="U1" s="21" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B2" s="9">
         <v>222482127286</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2">
+        <v>10</v>
+      </c>
+      <c r="I2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J2" s="2">
+        <v>3000</v>
+      </c>
+      <c r="K2" s="2">
+        <v>125</v>
+      </c>
+      <c r="L2" t="b">
+        <v>1</v>
+      </c>
+      <c r="O2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>75</v>
+      </c>
+      <c r="R2" t="s">
+        <v>76</v>
+      </c>
+      <c r="S2" t="s">
+        <v>77</v>
+      </c>
+      <c r="T2" t="s">
+        <v>78</v>
+      </c>
+      <c r="U2" s="2">
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F2" t="s">
-        <v>67</v>
-      </c>
-      <c r="G2">
-        <v>100</v>
-      </c>
-      <c r="H2" t="s">
-        <v>49</v>
-      </c>
-      <c r="I2" t="s">
-        <v>68</v>
-      </c>
-      <c r="J2" t="s">
-        <v>69</v>
-      </c>
-      <c r="K2">
-        <v>4000</v>
-      </c>
-      <c r="L2">
-        <v>250</v>
-      </c>
-      <c r="M2" t="b">
+      <c r="B3" s="9">
+        <v>222482127286</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H3">
+        <v>125</v>
+      </c>
+      <c r="I3" t="s">
+        <v>80</v>
+      </c>
+      <c r="J3" s="2">
+        <v>500</v>
+      </c>
+      <c r="K3" s="2">
+        <v>500</v>
+      </c>
+      <c r="L3" t="b">
         <v>1</v>
       </c>
-      <c r="P2" t="b">
+      <c r="O3" t="b">
         <v>0</v>
       </c>
-      <c r="Q2" t="str">
-        <f>_xlfn.XLOOKUP(E2,ec2_instances!F:F,ec2_instances!AG:AG)</f>
-        <v>hostname=az1autoprod-vm,solution=script_test</v>
+      <c r="Q3" t="s">
+        <v>75</v>
+      </c>
+      <c r="R3" t="s">
+        <v>81</v>
+      </c>
+      <c r="S3" t="s">
+        <v>82</v>
+      </c>
+      <c r="T3" t="s">
+        <v>78</v>
+      </c>
+      <c r="U3" s="2">
+        <v>65536</v>
       </c>
     </row>
   </sheetData>
@@ -1236,24 +1427,24 @@
         <v>4</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C2" s="9">
         <v>222482127286</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="E2" t="s">
-        <v>114</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1299,25 +1490,25 @@
         <v>3</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="L1" s="7" t="s">
         <v>32</v>
@@ -1325,78 +1516,78 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B2" s="2">
         <v>222482127286</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E2" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="F2" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="G2" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="H2">
         <v>5</v>
       </c>
       <c r="I2" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="J2" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="K2" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="L2" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B3" s="2">
         <v>222482127286</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E3" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="F3" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="G3" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="H3">
         <v>5</v>
       </c>
       <c r="I3" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="J3" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="K3" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="L3" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1444,31 +1635,31 @@
         <v>1</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="M1" s="4" t="s">
         <v>32</v>
@@ -1479,28 +1670,28 @@
     </row>
     <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B2" s="9">
         <v>222482127286</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>99</v>
+        <v>114</v>
       </c>
       <c r="I2" s="11">
         <v>80</v>
@@ -1509,42 +1700,42 @@
         <v>80</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="N2" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B3" s="9">
         <v>222482127286</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>99</v>
+        <v>114</v>
       </c>
       <c r="I3" s="11">
         <v>443</v>
@@ -1553,42 +1744,42 @@
         <v>443</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="N3" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B4" s="9">
         <v>222482127286</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>99</v>
+        <v>114</v>
       </c>
       <c r="I4" s="11">
         <v>22</v>
@@ -1597,42 +1788,42 @@
         <v>22</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="N4" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B5" s="9">
         <v>222482127286</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>99</v>
+        <v>114</v>
       </c>
       <c r="I5" s="11">
         <v>5723</v>
@@ -1641,16 +1832,16 @@
         <v>5723</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="N5" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1693,10 +1884,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>5</v>
@@ -1705,38 +1896,38 @@
         <v>4</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>106</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B2" s="9">
         <v>222482127286</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E2" t="str">
         <f>sg_rules!F2</f>
         <v>vpc-0b33c6cf3b601d4db</v>
       </c>
       <c r="F2" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="G2" t="str">
         <f>ec2_instances!F2</f>
         <v>az1autoprod-vm</v>
       </c>
       <c r="H2" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="I2" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1746,10 +1937,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{837A64A7-A28D-446B-BF65-8B5ADC476A37}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1776,50 +1967,55 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>122</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D2" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="B3" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>